<commit_message>
updated project files for workshop
</commit_message>
<xml_diff>
--- a/pathways data dictionary.xlsx
+++ b/pathways data dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/jeremy_cooper_gatesfoundation_org/Documents/Documents/GitHub/pathways-segmentation-public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2518" documentId="8_{D23518CC-E1D3-4ECE-9E98-7428ECDD5F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FC0D157-18D3-4156-A7B1-6024230B7060}"/>
+  <xr:revisionPtr revIDLastSave="2698" documentId="8_{D23518CC-E1D3-4ECE-9E98-7428ECDD5F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{460C35D4-A6ED-4FFA-B5A1-D59AB8DF36D1}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">outcomes!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">vulnerabilities!$A$1:$C$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">vulnerabilities!$A$1:$I$501</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="1698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="1769">
   <si>
     <t>category</t>
   </si>
@@ -5107,21 +5107,12 @@
     <t>Woman.and.her.past.experiences</t>
   </si>
   <si>
-    <t>Healthcare.and.mental.models</t>
-  </si>
-  <si>
     <t>Natural.and.human.systems</t>
   </si>
   <si>
     <t>Household.relationships</t>
   </si>
   <si>
-    <t>Household.economics</t>
-  </si>
-  <si>
-    <t>Community.Support</t>
-  </si>
-  <si>
     <t>Distance Natal</t>
   </si>
   <si>
@@ -5135,6 +5126,228 @@
   </si>
   <si>
     <t>HH Dropout</t>
+  </si>
+  <si>
+    <t>Social.support</t>
+  </si>
+  <si>
+    <t>Health.and.mental.models</t>
+  </si>
+  <si>
+    <t>conflict_incidents_26plus</t>
+  </si>
+  <si>
+    <t>Conflict Incidents 26 Plus</t>
+  </si>
+  <si>
+    <t>working.yn</t>
+  </si>
+  <si>
+    <t>partner.working.yn</t>
+  </si>
+  <si>
+    <t>Partner Working Y/N</t>
+  </si>
+  <si>
+    <t>pastoralnoagro.yn</t>
+  </si>
+  <si>
+    <t>Pastoral No Agro Y/N</t>
+  </si>
+  <si>
+    <t>hh.members</t>
+  </si>
+  <si>
+    <t>num.biochild.house</t>
+  </si>
+  <si>
+    <t>Num Bio Children House</t>
+  </si>
+  <si>
+    <t>num.biochild.house.cat</t>
+  </si>
+  <si>
+    <t>Num Bio Children House Cat</t>
+  </si>
+  <si>
+    <t>orthodox</t>
+  </si>
+  <si>
+    <t>Religion: Orthodox</t>
+  </si>
+  <si>
+    <t>partner.working</t>
+  </si>
+  <si>
+    <t>Partner Working</t>
+  </si>
+  <si>
+    <t>partner.workingnow.yn</t>
+  </si>
+  <si>
+    <t>wd.index.cat</t>
+  </si>
+  <si>
+    <t>Woman Decision Index Cat</t>
+  </si>
+  <si>
+    <t>Respondent Working Y/N</t>
+  </si>
+  <si>
+    <t>Household.economics.and.living.conditions</t>
+  </si>
+  <si>
+    <t>Differene between woman and male partner's preference for children</t>
+  </si>
+  <si>
+    <t>Has the respondent ever been  married</t>
+  </si>
+  <si>
+    <t>Does the household have cows</t>
+  </si>
+  <si>
+    <t>Does the household have chickens</t>
+  </si>
+  <si>
+    <t>Does the household have goats</t>
+  </si>
+  <si>
+    <t>Does the household have horses</t>
+  </si>
+  <si>
+    <t>Does the household have sheep</t>
+  </si>
+  <si>
+    <t>Household shares a latrine with another household (binary)</t>
+  </si>
+  <si>
+    <t>Household has internet</t>
+  </si>
+  <si>
+    <t>Husband's education level</t>
+  </si>
+  <si>
+    <t>Husband's education level less than primary</t>
+  </si>
+  <si>
+    <t>Husbands education level more than primary</t>
+  </si>
+  <si>
+    <t>Location of the household latrine</t>
+  </si>
+  <si>
+    <t>Male age at first birth</t>
+  </si>
+  <si>
+    <t>Reason for not seeking healthcare: does not know</t>
+  </si>
+  <si>
+    <t>Reason for not seeking healthcare</t>
+  </si>
+  <si>
+    <t>Household member count</t>
+  </si>
+  <si>
+    <t>Household members sleeping</t>
+  </si>
+  <si>
+    <t>Child given micronutrients in previous 12 months</t>
+  </si>
+  <si>
+    <t>Reads newspaper</t>
+  </si>
+  <si>
+    <t>Number of children over 15 years of age (binary 4+)</t>
+  </si>
+  <si>
+    <t>Number of children under 5 years of age (binary 2+)</t>
+  </si>
+  <si>
+    <t>Number of children alive category</t>
+  </si>
+  <si>
+    <t>Number of children that have died</t>
+  </si>
+  <si>
+    <t>Number of children that have died category</t>
+  </si>
+  <si>
+    <t>Binary variable for number of children that have died</t>
+  </si>
+  <si>
+    <t>Number of biological kids living in the home</t>
+  </si>
+  <si>
+    <t>Number of biological kids living in the home (binary 4+)</t>
+  </si>
+  <si>
+    <t>Categorical variable for number of biological kids living in the household</t>
+  </si>
+  <si>
+    <t>Frequency that child is given solid food</t>
+  </si>
+  <si>
+    <t>Number of household members under the age of 15 (binary 3+)</t>
+  </si>
+  <si>
+    <t>Respondent occupation</t>
+  </si>
+  <si>
+    <t>Partner currently working</t>
+  </si>
+  <si>
+    <t>Partner does not currently reside at home</t>
+  </si>
+  <si>
+    <t>Partner education level</t>
+  </si>
+  <si>
+    <t>Categorical variable for partner education level</t>
+  </si>
+  <si>
+    <t>Household water is piped</t>
+  </si>
+  <si>
+    <t>Respondent's current partnership status</t>
+  </si>
+  <si>
+    <t>Categorical variable for respondent's religion</t>
+  </si>
+  <si>
+    <t>Gifts for sex given in the previous 12 months</t>
+  </si>
+  <si>
+    <t>Household has a shared toilet</t>
+  </si>
+  <si>
+    <t>Slum categorical variable</t>
+  </si>
+  <si>
+    <t>Source of family planning information is government</t>
+  </si>
+  <si>
+    <t>Location of toilet</t>
+  </si>
+  <si>
+    <t>Household watches TV</t>
+  </si>
+  <si>
+    <t>Household has a solid wall</t>
+  </si>
+  <si>
+    <t>Number of household members</t>
+  </si>
+  <si>
+    <t>Number biological children in household</t>
+  </si>
+  <si>
+    <t>Number biological children in household category</t>
+  </si>
+  <si>
+    <t>Respondent is of Orthodox faith</t>
+  </si>
+  <si>
+    <t>Categorical variable for woman decision making index</t>
   </si>
 </sst>
 </file>
@@ -7292,18 +7505,18 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:I490"/>
+  <dimension ref="A1:I501"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A468" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D491" sqref="D491"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C500" sqref="C500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
     <col min="4" max="4" width="28.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.26953125" bestFit="1" customWidth="1"/>
@@ -7326,19 +7539,19 @@
         <v>1687</v>
       </c>
       <c r="E1" t="s">
+        <v>1696</v>
+      </c>
+      <c r="F1" t="s">
         <v>1688</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1689</v>
       </c>
-      <c r="G1" t="s">
-        <v>1690</v>
-      </c>
       <c r="H1" t="s">
-        <v>1691</v>
+        <v>1717</v>
       </c>
       <c r="I1" t="s">
-        <v>1692</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -7908,6 +8121,9 @@
       <c r="B42" t="s">
         <v>1661</v>
       </c>
+      <c r="C42" t="s">
+        <v>1718</v>
+      </c>
       <c r="D42">
         <v>1</v>
       </c>
@@ -8407,7 +8623,7 @@
         <v>1249</v>
       </c>
       <c r="B78" t="s">
-        <v>1693</v>
+        <v>1690</v>
       </c>
       <c r="C78" t="s">
         <v>1250</v>
@@ -8421,7 +8637,7 @@
         <v>1074</v>
       </c>
       <c r="B79" t="s">
-        <v>1694</v>
+        <v>1691</v>
       </c>
       <c r="C79" t="s">
         <v>1075</v>
@@ -9277,6 +9493,9 @@
       <c r="B140" t="s">
         <v>1666</v>
       </c>
+      <c r="C140" t="s">
+        <v>1719</v>
+      </c>
       <c r="G140">
         <v>1</v>
       </c>
@@ -9594,7 +9813,7 @@
         <v>1168</v>
       </c>
       <c r="B163" t="s">
-        <v>1695</v>
+        <v>1692</v>
       </c>
       <c r="C163" t="s">
         <v>1169</v>
@@ -9641,7 +9860,7 @@
       <c r="C166" t="s">
         <v>219</v>
       </c>
-      <c r="F166">
+      <c r="H166">
         <v>1</v>
       </c>
     </row>
@@ -9694,7 +9913,7 @@
       <c r="C170" t="s">
         <v>226</v>
       </c>
-      <c r="F170">
+      <c r="H170">
         <v>1</v>
       </c>
     </row>
@@ -9744,7 +9963,7 @@
       <c r="C174" t="s">
         <v>643</v>
       </c>
-      <c r="F174">
+      <c r="H174">
         <v>1</v>
       </c>
     </row>
@@ -9758,7 +9977,7 @@
       <c r="C175" t="s">
         <v>645</v>
       </c>
-      <c r="F175">
+      <c r="H175">
         <v>1</v>
       </c>
     </row>
@@ -9772,7 +9991,7 @@
       <c r="C176" t="s">
         <v>648</v>
       </c>
-      <c r="F176">
+      <c r="H176">
         <v>1</v>
       </c>
     </row>
@@ -9783,7 +10002,10 @@
       <c r="B177" t="s">
         <v>1686</v>
       </c>
-      <c r="F177">
+      <c r="C177" t="s">
+        <v>1720</v>
+      </c>
+      <c r="H177">
         <v>1</v>
       </c>
     </row>
@@ -9794,7 +10016,10 @@
       <c r="B178" t="s">
         <v>1668</v>
       </c>
-      <c r="F178">
+      <c r="C178" t="s">
+        <v>1721</v>
+      </c>
+      <c r="H178">
         <v>1</v>
       </c>
     </row>
@@ -9805,7 +10030,10 @@
       <c r="B179" t="s">
         <v>1670</v>
       </c>
-      <c r="F179">
+      <c r="C179" t="s">
+        <v>1722</v>
+      </c>
+      <c r="H179">
         <v>1</v>
       </c>
     </row>
@@ -9816,7 +10044,10 @@
       <c r="B180" t="s">
         <v>1672</v>
       </c>
-      <c r="F180">
+      <c r="C180" t="s">
+        <v>1723</v>
+      </c>
+      <c r="H180">
         <v>1</v>
       </c>
     </row>
@@ -9827,7 +10058,10 @@
       <c r="B181" t="s">
         <v>1675</v>
       </c>
-      <c r="F181">
+      <c r="C181" t="s">
+        <v>1724</v>
+      </c>
+      <c r="H181">
         <v>1</v>
       </c>
     </row>
@@ -9838,6 +10072,9 @@
       <c r="B182" t="s">
         <v>1529</v>
       </c>
+      <c r="C182" t="s">
+        <v>1725</v>
+      </c>
       <c r="F182">
         <v>1</v>
       </c>
@@ -9847,7 +10084,7 @@
         <v>1108</v>
       </c>
       <c r="B183" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="C183" t="s">
         <v>1109</v>
@@ -9917,7 +10154,7 @@
         <v>1110</v>
       </c>
       <c r="B188" t="s">
-        <v>1697</v>
+        <v>1694</v>
       </c>
       <c r="C188" t="s">
         <v>1111</v>
@@ -10003,6 +10240,9 @@
       <c r="B194" t="s">
         <v>1033</v>
       </c>
+      <c r="C194" t="s">
+        <v>1726</v>
+      </c>
       <c r="F194">
         <v>1</v>
       </c>
@@ -10952,6 +11192,9 @@
       <c r="B262" t="s">
         <v>727</v>
       </c>
+      <c r="C262" t="s">
+        <v>1727</v>
+      </c>
       <c r="G262">
         <v>1</v>
       </c>
@@ -10963,6 +11206,9 @@
       <c r="B263" t="s">
         <v>731</v>
       </c>
+      <c r="C263" t="s">
+        <v>1728</v>
+      </c>
       <c r="G263">
         <v>1</v>
       </c>
@@ -10974,6 +11220,9 @@
       <c r="B264" t="s">
         <v>729</v>
       </c>
+      <c r="C264" t="s">
+        <v>1729</v>
+      </c>
       <c r="G264">
         <v>1</v>
       </c>
@@ -11601,6 +11850,9 @@
       <c r="B309" t="s">
         <v>1677</v>
       </c>
+      <c r="C309" t="s">
+        <v>1730</v>
+      </c>
       <c r="F309">
         <v>1</v>
       </c>
@@ -11637,6 +11889,9 @@
       <c r="B312" t="s">
         <v>1551</v>
       </c>
+      <c r="C312" t="s">
+        <v>1731</v>
+      </c>
       <c r="G312">
         <v>1</v>
       </c>
@@ -11858,6 +12113,9 @@
       <c r="B328" t="s">
         <v>1564</v>
       </c>
+      <c r="C328" t="s">
+        <v>1732</v>
+      </c>
       <c r="E328">
         <v>1</v>
       </c>
@@ -11869,6 +12127,9 @@
       <c r="B329" t="s">
         <v>1565</v>
       </c>
+      <c r="C329" t="s">
+        <v>1733</v>
+      </c>
       <c r="E329">
         <v>1</v>
       </c>
@@ -11908,6 +12169,9 @@
       <c r="B332" t="s">
         <v>1567</v>
       </c>
+      <c r="C332" t="s">
+        <v>1733</v>
+      </c>
       <c r="E332">
         <v>1</v>
       </c>
@@ -11933,6 +12197,9 @@
       <c r="B334" t="s">
         <v>1569</v>
       </c>
+      <c r="C334" t="s">
+        <v>1733</v>
+      </c>
       <c r="E334">
         <v>1</v>
       </c>
@@ -11944,6 +12211,9 @@
       <c r="B335" t="s">
         <v>1570</v>
       </c>
+      <c r="C335" t="s">
+        <v>1733</v>
+      </c>
       <c r="E335">
         <v>1</v>
       </c>
@@ -11955,6 +12225,9 @@
       <c r="B336" t="s">
         <v>1571</v>
       </c>
+      <c r="C336" t="s">
+        <v>1733</v>
+      </c>
       <c r="E336">
         <v>1</v>
       </c>
@@ -11994,6 +12267,9 @@
       <c r="B339" t="s">
         <v>1572</v>
       </c>
+      <c r="C339" t="s">
+        <v>1733</v>
+      </c>
       <c r="E339">
         <v>1</v>
       </c>
@@ -12033,6 +12309,9 @@
       <c r="B342" t="s">
         <v>1575</v>
       </c>
+      <c r="C342" t="s">
+        <v>1734</v>
+      </c>
       <c r="G342">
         <v>1</v>
       </c>
@@ -12044,6 +12323,9 @@
       <c r="B343" t="s">
         <v>1576</v>
       </c>
+      <c r="C343" t="s">
+        <v>1735</v>
+      </c>
       <c r="G343">
         <v>1</v>
       </c>
@@ -12055,6 +12337,9 @@
       <c r="B344" t="s">
         <v>1577</v>
       </c>
+      <c r="C344" t="s">
+        <v>1736</v>
+      </c>
       <c r="E344">
         <v>1</v>
       </c>
@@ -12186,6 +12471,9 @@
       <c r="B354" t="s">
         <v>1583</v>
       </c>
+      <c r="C354" t="s">
+        <v>1737</v>
+      </c>
       <c r="H354">
         <v>1</v>
       </c>
@@ -12309,6 +12597,9 @@
       <c r="B363" t="s">
         <v>1584</v>
       </c>
+      <c r="C363" t="s">
+        <v>1738</v>
+      </c>
       <c r="G363">
         <v>1</v>
       </c>
@@ -12362,6 +12653,9 @@
       <c r="B367" t="s">
         <v>1590</v>
       </c>
+      <c r="C367" t="s">
+        <v>1740</v>
+      </c>
       <c r="G367">
         <v>1</v>
       </c>
@@ -12373,6 +12667,9 @@
       <c r="B368" t="s">
         <v>1591</v>
       </c>
+      <c r="C368" t="s">
+        <v>1741</v>
+      </c>
       <c r="G368">
         <v>1</v>
       </c>
@@ -12384,6 +12681,9 @@
       <c r="B369" t="s">
         <v>1592</v>
       </c>
+      <c r="C369" t="s">
+        <v>1742</v>
+      </c>
       <c r="G369">
         <v>1</v>
       </c>
@@ -12395,6 +12695,9 @@
       <c r="B370" t="s">
         <v>1593</v>
       </c>
+      <c r="C370" t="s">
+        <v>1743</v>
+      </c>
       <c r="G370">
         <v>1</v>
       </c>
@@ -12406,6 +12709,9 @@
       <c r="B371" t="s">
         <v>1588</v>
       </c>
+      <c r="C371" t="s">
+        <v>1744</v>
+      </c>
       <c r="G371">
         <v>1</v>
       </c>
@@ -12417,6 +12723,9 @@
       <c r="B372" t="s">
         <v>1586</v>
       </c>
+      <c r="C372" t="s">
+        <v>1745</v>
+      </c>
       <c r="G372">
         <v>1</v>
       </c>
@@ -12428,6 +12737,9 @@
       <c r="B373" t="s">
         <v>1589</v>
       </c>
+      <c r="C373" t="s">
+        <v>1746</v>
+      </c>
       <c r="G373">
         <v>1</v>
       </c>
@@ -12481,6 +12793,9 @@
       <c r="B377" t="s">
         <v>1594</v>
       </c>
+      <c r="C377" t="s">
+        <v>1747</v>
+      </c>
       <c r="E377">
         <v>1</v>
       </c>
@@ -12506,6 +12821,9 @@
       <c r="B379" t="s">
         <v>1595</v>
       </c>
+      <c r="C379" t="s">
+        <v>1748</v>
+      </c>
       <c r="G379">
         <v>1</v>
       </c>
@@ -12545,6 +12863,9 @@
       <c r="B382" t="s">
         <v>1596</v>
       </c>
+      <c r="C382" t="s">
+        <v>1739</v>
+      </c>
       <c r="G382">
         <v>1</v>
       </c>
@@ -12584,6 +12905,9 @@
       <c r="B385" t="s">
         <v>1597</v>
       </c>
+      <c r="C385" t="s">
+        <v>1749</v>
+      </c>
       <c r="G385">
         <v>1</v>
       </c>
@@ -12609,6 +12933,9 @@
       <c r="B387" t="s">
         <v>1598</v>
       </c>
+      <c r="C387" t="s">
+        <v>1750</v>
+      </c>
       <c r="G387">
         <v>1</v>
       </c>
@@ -12620,6 +12947,9 @@
       <c r="B388" t="s">
         <v>1598</v>
       </c>
+      <c r="C388" t="s">
+        <v>1750</v>
+      </c>
       <c r="G388">
         <v>1</v>
       </c>
@@ -12645,6 +12975,9 @@
       <c r="B390" t="s">
         <v>1599</v>
       </c>
+      <c r="C390" t="s">
+        <v>1751</v>
+      </c>
       <c r="G390">
         <v>1</v>
       </c>
@@ -12726,6 +13059,9 @@
       <c r="B396" t="s">
         <v>1039</v>
       </c>
+      <c r="C396" t="s">
+        <v>1752</v>
+      </c>
       <c r="G396">
         <v>1</v>
       </c>
@@ -12737,6 +13073,9 @@
       <c r="B397" t="s">
         <v>1680</v>
       </c>
+      <c r="C397" t="s">
+        <v>1753</v>
+      </c>
       <c r="G397">
         <v>1</v>
       </c>
@@ -12748,6 +13087,9 @@
       <c r="B398" t="s">
         <v>1683</v>
       </c>
+      <c r="C398" t="s">
+        <v>1753</v>
+      </c>
       <c r="G398">
         <v>1</v>
       </c>
@@ -12857,6 +13199,9 @@
       <c r="B406" t="s">
         <v>1604</v>
       </c>
+      <c r="C406" t="s">
+        <v>1754</v>
+      </c>
       <c r="F406">
         <v>1</v>
       </c>
@@ -12960,6 +13305,9 @@
       <c r="B414" t="s">
         <v>1608</v>
       </c>
+      <c r="C414" t="s">
+        <v>955</v>
+      </c>
       <c r="D414">
         <v>1</v>
       </c>
@@ -12971,6 +13319,9 @@
       <c r="B415" t="s">
         <v>1609</v>
       </c>
+      <c r="C415" t="s">
+        <v>1755</v>
+      </c>
       <c r="D415">
         <v>1</v>
       </c>
@@ -13018,6 +13369,9 @@
       <c r="B419" t="s">
         <v>1612</v>
       </c>
+      <c r="C419" t="s">
+        <v>1756</v>
+      </c>
       <c r="D419">
         <v>1</v>
       </c>
@@ -13057,6 +13411,9 @@
       <c r="B422" t="s">
         <v>1615</v>
       </c>
+      <c r="C422" t="s">
+        <v>1757</v>
+      </c>
       <c r="D422">
         <v>1</v>
       </c>
@@ -13068,6 +13425,9 @@
       <c r="B423" t="s">
         <v>1616</v>
       </c>
+      <c r="C423" t="s">
+        <v>1758</v>
+      </c>
       <c r="F423">
         <v>1</v>
       </c>
@@ -13107,6 +13467,9 @@
       <c r="B426" t="s">
         <v>1618</v>
       </c>
+      <c r="C426" t="s">
+        <v>1759</v>
+      </c>
       <c r="F426">
         <v>1</v>
       </c>
@@ -13118,6 +13481,9 @@
       <c r="B427" t="s">
         <v>1619</v>
       </c>
+      <c r="C427" t="s">
+        <v>1759</v>
+      </c>
       <c r="F427">
         <v>1</v>
       </c>
@@ -13143,6 +13509,9 @@
       <c r="B429" t="s">
         <v>1621</v>
       </c>
+      <c r="C429" t="s">
+        <v>1760</v>
+      </c>
       <c r="E429">
         <v>1</v>
       </c>
@@ -13176,6 +13545,9 @@
       <c r="B432" t="s">
         <v>1623</v>
       </c>
+      <c r="C432" t="s">
+        <v>1761</v>
+      </c>
       <c r="F432">
         <v>1</v>
       </c>
@@ -13201,6 +13573,9 @@
       <c r="B434" t="s">
         <v>1625</v>
       </c>
+      <c r="C434" t="s">
+        <v>1761</v>
+      </c>
       <c r="F434">
         <v>1</v>
       </c>
@@ -13338,6 +13713,9 @@
       <c r="B444" t="s">
         <v>1038</v>
       </c>
+      <c r="C444" t="s">
+        <v>1762</v>
+      </c>
       <c r="H444">
         <v>1</v>
       </c>
@@ -13416,6 +13794,9 @@
       <c r="B450" t="s">
         <v>1639</v>
       </c>
+      <c r="C450" t="s">
+        <v>1763</v>
+      </c>
       <c r="F450">
         <v>1</v>
       </c>
@@ -13872,7 +14253,7 @@
       <c r="C483" t="s">
         <v>455</v>
       </c>
-      <c r="D483">
+      <c r="H483">
         <v>1</v>
       </c>
     </row>
@@ -13886,7 +14267,7 @@
       <c r="C484" t="s">
         <v>1128</v>
       </c>
-      <c r="D484">
+      <c r="H484">
         <v>1</v>
       </c>
     </row>
@@ -13900,7 +14281,7 @@
       <c r="C485" t="s">
         <v>1130</v>
       </c>
-      <c r="D485">
+      <c r="H485">
         <v>1</v>
       </c>
     </row>
@@ -13914,7 +14295,7 @@
       <c r="C486" t="s">
         <v>1054</v>
       </c>
-      <c r="D486">
+      <c r="H486">
         <v>1</v>
       </c>
     </row>
@@ -13928,7 +14309,7 @@
       <c r="C487" t="s">
         <v>953</v>
       </c>
-      <c r="D487">
+      <c r="H487">
         <v>1</v>
       </c>
     </row>
@@ -13942,7 +14323,7 @@
       <c r="C488" t="s">
         <v>459</v>
       </c>
-      <c r="D488">
+      <c r="H488">
         <v>1</v>
       </c>
     </row>
@@ -13974,12 +14355,156 @@
         <v>1</v>
       </c>
     </row>
+    <row r="491" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A491" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B491" t="s">
+        <v>1698</v>
+      </c>
+      <c r="G491">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="492" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A492" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B492" t="s">
+        <v>1703</v>
+      </c>
+      <c r="F492">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="493" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A493" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B493" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C493" t="s">
+        <v>1764</v>
+      </c>
+      <c r="G493">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="494" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A494" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B494" t="s">
+        <v>1706</v>
+      </c>
+      <c r="C494" t="s">
+        <v>1765</v>
+      </c>
+      <c r="G494">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A495" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B495" t="s">
+        <v>1708</v>
+      </c>
+      <c r="C495" t="s">
+        <v>1766</v>
+      </c>
+      <c r="G495">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A496" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B496" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C496" t="s">
+        <v>1767</v>
+      </c>
+      <c r="D496">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A497" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B497" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C497" t="s">
+        <v>1750</v>
+      </c>
+      <c r="H497">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A498" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B498" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C498" t="s">
+        <v>1750</v>
+      </c>
+      <c r="H498">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A499" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B499" t="s">
+        <v>414</v>
+      </c>
+      <c r="C499" t="s">
+        <v>1750</v>
+      </c>
+      <c r="H499">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A500" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B500" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C500" t="s">
+        <v>1768</v>
+      </c>
+      <c r="G500">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A501" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B501" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C501" t="s">
+        <v>459</v>
+      </c>
+      <c r="H501">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C354" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C491">
-      <sortCondition ref="A1:A354"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:I501" xr:uid="{00000000-0001-0000-0B00-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>